<commit_message>
added functionality for different types of invoices
</commit_message>
<xml_diff>
--- a/resources/report.xlsx
+++ b/resources/report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianguarino/projects/invoice_generator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9C7A9C-17B4-A44F-BC6F-90F49AAFC7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F312744-FAB6-C242-94D1-AD6AFA43C570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="3120" windowWidth="12980" windowHeight="15380" firstSheet="13" activeTab="19" xr2:uid="{4B2E9ECB-EC2D-4112-A2A1-931DBA23B9A7}"/>
+    <workbookView xWindow="16700" yWindow="3120" windowWidth="12980" windowHeight="15380" firstSheet="14" activeTab="19" xr2:uid="{4B2E9ECB-EC2D-4112-A2A1-931DBA23B9A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 22" sheetId="50" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="183">
   <si>
     <t>UNIT</t>
   </si>
@@ -594,10 +594,16 @@
     <t>2406F</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -632,7 +638,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -655,11 +661,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,6 +712,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5344,7 +5364,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5352,7 +5372,7 @@
     <col min="2" max="2" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5368,8 +5388,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>210</v>
       </c>
@@ -5383,8 +5406,11 @@
       <c r="E2" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>214</v>
       </c>
@@ -5398,8 +5424,11 @@
       <c r="E3" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>215</v>
       </c>
@@ -5413,8 +5442,11 @@
       <c r="E4" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>217</v>
       </c>
@@ -5428,8 +5460,11 @@
       <c r="E5" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>308</v>
       </c>
@@ -5443,8 +5478,11 @@
       <c r="E6" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>314</v>
       </c>
@@ -5458,8 +5496,11 @@
       <c r="E7" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>402</v>
       </c>
@@ -5473,8 +5514,11 @@
       <c r="E8" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>405</v>
       </c>
@@ -5488,8 +5532,11 @@
       <c r="E9" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>407</v>
       </c>
@@ -5503,8 +5550,11 @@
       <c r="E10" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>412</v>
       </c>
@@ -5518,8 +5568,11 @@
       <c r="E11" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>413</v>
       </c>
@@ -5533,8 +5586,11 @@
       <c r="E12" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>414</v>
       </c>
@@ -5548,8 +5604,11 @@
       <c r="E13" s="6">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>414</v>
       </c>
@@ -5563,8 +5622,11 @@
       <c r="E14" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>416</v>
       </c>
@@ -5578,8 +5640,11 @@
       <c r="E15" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>502</v>
       </c>
@@ -5593,8 +5658,11 @@
       <c r="E16" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>503</v>
       </c>
@@ -5608,8 +5676,11 @@
       <c r="E17" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>504</v>
       </c>
@@ -5623,8 +5694,11 @@
       <c r="E18" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>507</v>
       </c>
@@ -5638,8 +5712,11 @@
       <c r="E19" s="6">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>507</v>
       </c>
@@ -5653,8 +5730,11 @@
       <c r="E20" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>508</v>
       </c>
@@ -5668,8 +5748,11 @@
       <c r="E21" s="6">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>509</v>
       </c>
@@ -5683,8 +5766,11 @@
       <c r="E22" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>512</v>
       </c>
@@ -5698,8 +5784,11 @@
       <c r="E23" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>513</v>
       </c>
@@ -5713,8 +5802,11 @@
       <c r="E24" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>522</v>
       </c>
@@ -5728,8 +5820,11 @@
       <c r="E25" s="6">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>602</v>
       </c>
@@ -5743,8 +5838,11 @@
       <c r="E26" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>603</v>
       </c>
@@ -5758,8 +5856,11 @@
       <c r="E27" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>604</v>
       </c>
@@ -5773,8 +5874,11 @@
       <c r="E28" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>607</v>
       </c>
@@ -5788,8 +5892,11 @@
       <c r="E29" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>608</v>
       </c>
@@ -5803,8 +5910,11 @@
       <c r="E30" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>612</v>
       </c>
@@ -5818,8 +5928,11 @@
       <c r="E31" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>615</v>
       </c>
@@ -5833,8 +5946,11 @@
       <c r="E32" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>703</v>
       </c>
@@ -5848,8 +5964,11 @@
       <c r="E33" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>709</v>
       </c>
@@ -5863,8 +5982,11 @@
       <c r="E34" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>802</v>
       </c>
@@ -5878,8 +6000,11 @@
       <c r="E35" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>803</v>
       </c>
@@ -5893,8 +6018,11 @@
       <c r="E36" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>806</v>
       </c>
@@ -5908,8 +6036,11 @@
       <c r="E37" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>809</v>
       </c>
@@ -5923,8 +6054,11 @@
         <v>10</v>
       </c>
       <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>905</v>
       </c>
@@ -5938,8 +6072,11 @@
       <c r="E39" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>1002</v>
       </c>
@@ -5953,8 +6090,11 @@
       <c r="E40" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>1006</v>
       </c>
@@ -5968,8 +6108,11 @@
       <c r="E41" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>1206</v>
       </c>
@@ -5983,8 +6126,11 @@
       <c r="E42" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>1207</v>
       </c>
@@ -5998,8 +6144,11 @@
       <c r="E43" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>1208</v>
       </c>
@@ -6013,8 +6162,11 @@
       <c r="E44" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>1301</v>
       </c>
@@ -6028,8 +6180,11 @@
       <c r="E45" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>1309</v>
       </c>
@@ -6043,8 +6198,11 @@
       <c r="E46" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>1401</v>
       </c>
@@ -6058,8 +6216,11 @@
       <c r="E47" s="6">
         <v>75</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>1402</v>
       </c>
@@ -6073,8 +6234,11 @@
       <c r="E48" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>1403</v>
       </c>
@@ -6088,8 +6252,11 @@
       <c r="E49" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>1404</v>
       </c>
@@ -6103,8 +6270,11 @@
       <c r="E50" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>1405</v>
       </c>
@@ -6118,8 +6288,11 @@
       <c r="E51" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>1409</v>
       </c>
@@ -6133,8 +6306,11 @@
       <c r="E52" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>1422</v>
       </c>
@@ -6148,8 +6324,11 @@
       <c r="E53" s="6">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>1502</v>
       </c>
@@ -6163,8 +6342,11 @@
       <c r="E54" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>1504</v>
       </c>
@@ -6178,8 +6360,11 @@
       <c r="E55" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>1603</v>
       </c>
@@ -6193,8 +6378,11 @@
       <c r="E56" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>1604</v>
       </c>
@@ -6208,8 +6396,11 @@
       <c r="E57" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>1606</v>
       </c>
@@ -6223,8 +6414,11 @@
       <c r="E58" s="6">
         <v>200</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>1708</v>
       </c>
@@ -6238,8 +6432,11 @@
       <c r="E59" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>1709</v>
       </c>
@@ -6253,8 +6450,11 @@
       <c r="E60" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>1803</v>
       </c>
@@ -6268,8 +6468,11 @@
       <c r="E61" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>1807</v>
       </c>
@@ -6283,8 +6486,11 @@
       <c r="E62" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>1809</v>
       </c>
@@ -6298,8 +6504,11 @@
       <c r="E63" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>1922</v>
       </c>
@@ -6313,6 +6522,9 @@
       <c r="E64" s="6">
         <v>100</v>
       </c>
+      <c r="F64" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
@@ -6328,6 +6540,9 @@
       <c r="E65" s="6">
         <v>75</v>
       </c>
+      <c r="F65" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
@@ -6343,6 +6558,9 @@
       <c r="E66" s="6">
         <v>75</v>
       </c>
+      <c r="F66" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
@@ -6358,6 +6576,9 @@
       <c r="E67" s="6">
         <v>80</v>
       </c>
+      <c r="F67" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
@@ -6373,6 +6594,9 @@
       <c r="E68" s="6">
         <v>85</v>
       </c>
+      <c r="F68" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
@@ -6388,6 +6612,9 @@
       <c r="E69" s="6">
         <v>80</v>
       </c>
+      <c r="F69" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
@@ -6403,6 +6630,9 @@
       <c r="E70" s="6">
         <v>85</v>
       </c>
+      <c r="F70" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
@@ -6418,6 +6648,9 @@
       <c r="E71" s="6">
         <v>80</v>
       </c>
+      <c r="F71" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
@@ -6433,6 +6666,9 @@
       <c r="E72" s="6">
         <v>85</v>
       </c>
+      <c r="F72" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
@@ -6448,6 +6684,9 @@
       <c r="E73" s="6">
         <v>80</v>
       </c>
+      <c r="F73" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
@@ -6463,6 +6702,9 @@
       <c r="E74" s="6">
         <v>80</v>
       </c>
+      <c r="F74" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
@@ -6478,6 +6720,9 @@
       <c r="E75" s="6">
         <v>85</v>
       </c>
+      <c r="F75" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
@@ -6493,6 +6738,9 @@
       <c r="E76" s="6">
         <v>80</v>
       </c>
+      <c r="F76" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
@@ -6507,6 +6755,9 @@
       <c r="D77" s="6"/>
       <c r="E77" s="6">
         <v>85</v>
+      </c>
+      <c r="F77" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -6531,7 +6782,7 @@
         <v>85</v>
       </c>
       <c r="F79" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -6549,7 +6800,7 @@
         <v>75</v>
       </c>
       <c r="F80" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -6567,7 +6818,7 @@
         <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -6584,6 +6835,9 @@
       <c r="E82" s="6">
         <v>100</v>
       </c>
+      <c r="F82" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
@@ -6599,6 +6853,9 @@
       <c r="E83" s="6">
         <v>75</v>
       </c>
+      <c r="F83" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
@@ -6615,6 +6872,9 @@
       </c>
       <c r="E84" s="6">
         <v>75</v>
+      </c>
+      <c r="F84" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -10290,17 +10550,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27a4c553-e118-4eca-8f68-9ab2f6bc7790">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="072f65fd-8ac8-4458-b326-98f31ae95622" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056AE81D6219DD048908ADF242EEFC32D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8986bdc60267b136fae45e9c5006776b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="072f65fd-8ac8-4458-b326-98f31ae95622" xmlns:ns3="27a4c553-e118-4eca-8f68-9ab2f6bc7790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3fc11a8a20b827f47d265a4e041875c3" ns2:_="" ns3:_="">
     <xsd:import namespace="072f65fd-8ac8-4458-b326-98f31ae95622"/>
@@ -10535,6 +10784,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27a4c553-e118-4eca-8f68-9ab2f6bc7790">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="072f65fd-8ac8-4458-b326-98f31ae95622" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3F43D9-F9A1-4725-A9B7-C5F5F2B8D269}">
   <ds:schemaRefs>
@@ -10544,17 +10804,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2BB9A02-9680-4F30-A06C-9579F93AE1D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27a4c553-e118-4eca-8f68-9ab2f6bc7790"/>
-    <ds:schemaRef ds:uri="072f65fd-8ac8-4458-b326-98f31ae95622"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F96BD55E-408A-4963-8C68-986ACBD01E62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10571,4 +10820,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2BB9A02-9680-4F30-A06C-9579F93AE1D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27a4c553-e118-4eca-8f68-9ab2f6bc7790"/>
+    <ds:schemaRef ds:uri="072f65fd-8ac8-4458-b326-98f31ae95622"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added screenshots and more proofreading
</commit_message>
<xml_diff>
--- a/resources/report.xlsx
+++ b/resources/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianguarino/projects/invoice_generator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F312744-FAB6-C242-94D1-AD6AFA43C570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD67808-7573-B545-A25B-FF85447A6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="3120" windowWidth="12980" windowHeight="15380" firstSheet="14" activeTab="19" xr2:uid="{4B2E9ECB-EC2D-4112-A2A1-931DBA23B9A7}"/>
+    <workbookView xWindow="27260" yWindow="3340" windowWidth="12980" windowHeight="15380" firstSheet="14" activeTab="19" xr2:uid="{4B2E9ECB-EC2D-4112-A2A1-931DBA23B9A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 22" sheetId="50" r:id="rId1"/>
@@ -714,7 +714,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5363,7 +5363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869D5DDF-C373-4BF3-B66A-904044A0B34D}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -10541,15 +10541,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056AE81D6219DD048908ADF242EEFC32D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8986bdc60267b136fae45e9c5006776b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="072f65fd-8ac8-4458-b326-98f31ae95622" xmlns:ns3="27a4c553-e118-4eca-8f68-9ab2f6bc7790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3fc11a8a20b827f47d265a4e041875c3" ns2:_="" ns3:_="">
     <xsd:import namespace="072f65fd-8ac8-4458-b326-98f31ae95622"/>
@@ -10784,6 +10775,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -10796,14 +10796,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3F43D9-F9A1-4725-A9B7-C5F5F2B8D269}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F96BD55E-408A-4963-8C68-986ACBD01E62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10822,6 +10814,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3F43D9-F9A1-4725-A9B7-C5F5F2B8D269}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2BB9A02-9680-4F30-A06C-9579F93AE1D8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix: generate new folder for pdfs based on current month. + OCD
</commit_message>
<xml_diff>
--- a/resources/report.xlsx
+++ b/resources/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianguarino/projects/invoice_generator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD67808-7573-B545-A25B-FF85447A6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A4268-78F9-AA48-B62B-294345389D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27260" yWindow="3340" windowWidth="12980" windowHeight="15380" firstSheet="14" activeTab="19" xr2:uid="{4B2E9ECB-EC2D-4112-A2A1-931DBA23B9A7}"/>
+    <workbookView xWindow="25600" yWindow="780" windowWidth="25600" windowHeight="20220" firstSheet="14" activeTab="19" xr2:uid="{4B2E9ECB-EC2D-4112-A2A1-931DBA23B9A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 22" sheetId="50" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="185">
   <si>
     <t>UNIT</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>PARTS</t>
+  </si>
+  <si>
+    <t>LABOR</t>
   </si>
 </sst>
 </file>
@@ -669,14 +675,16 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -714,7 +722,13 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5363,9 +5377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869D5DDF-C373-4BF3-B66A-904044A0B34D}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5383,12 +5395,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5406,7 +5418,7 @@
       <c r="E2" s="6">
         <v>80</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5424,7 +5436,7 @@
       <c r="E3" s="6">
         <v>80</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5442,7 +5454,7 @@
       <c r="E4" s="6">
         <v>80</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5460,7 +5472,7 @@
       <c r="E5" s="6">
         <v>80</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5478,7 +5490,7 @@
       <c r="E6" s="6">
         <v>80</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5496,7 +5508,7 @@
       <c r="E7" s="6">
         <v>80</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5514,7 +5526,7 @@
       <c r="E8" s="6">
         <v>80</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5532,7 +5544,7 @@
       <c r="E9" s="6">
         <v>80</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5550,7 +5562,7 @@
       <c r="E10" s="6">
         <v>80</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5568,7 +5580,7 @@
       <c r="E11" s="6">
         <v>80</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5586,7 +5598,7 @@
       <c r="E12" s="6">
         <v>80</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5604,7 +5616,7 @@
       <c r="E13" s="6">
         <v>75</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5622,7 +5634,7 @@
       <c r="E14" s="6">
         <v>80</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5640,7 +5652,7 @@
       <c r="E15" s="6">
         <v>80</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5658,7 +5670,7 @@
       <c r="E16" s="6">
         <v>85</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5676,7 +5688,7 @@
       <c r="E17" s="6">
         <v>80</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5694,7 +5706,7 @@
       <c r="E18" s="6">
         <v>85</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5712,7 +5724,7 @@
       <c r="E19" s="6">
         <v>75</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5730,7 +5742,7 @@
       <c r="E20" s="6">
         <v>80</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5748,7 +5760,7 @@
       <c r="E21" s="6">
         <v>75</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5766,7 +5778,7 @@
       <c r="E22" s="6">
         <v>85</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5784,7 +5796,7 @@
       <c r="E23" s="6">
         <v>80</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5802,7 +5814,7 @@
       <c r="E24" s="6">
         <v>80</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5820,7 +5832,7 @@
       <c r="E25" s="6">
         <v>75</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5838,7 +5850,7 @@
       <c r="E26" s="6">
         <v>80</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5856,7 +5868,7 @@
       <c r="E27" s="6">
         <v>80</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5874,7 +5886,7 @@
       <c r="E28" s="6">
         <v>85</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5892,7 +5904,7 @@
       <c r="E29" s="6">
         <v>80</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5910,7 +5922,7 @@
       <c r="E30" s="6">
         <v>80</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5928,7 +5940,7 @@
       <c r="E31" s="6">
         <v>80</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5946,7 +5958,7 @@
       <c r="E32" s="6">
         <v>80</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5964,7 +5976,7 @@
       <c r="E33" s="6">
         <v>80</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5982,7 +5994,7 @@
       <c r="E34" s="6">
         <v>85</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6000,7 +6012,7 @@
       <c r="E35" s="6">
         <v>85</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6018,7 +6030,7 @@
       <c r="E36" s="6">
         <v>80</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6036,7 +6048,7 @@
       <c r="E37" s="6">
         <v>85</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6054,7 +6066,7 @@
         <v>10</v>
       </c>
       <c r="E38" s="6"/>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6072,7 +6084,7 @@
       <c r="E39" s="6">
         <v>85</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6090,7 +6102,7 @@
       <c r="E40" s="6">
         <v>80</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6108,7 +6120,7 @@
       <c r="E41" s="6">
         <v>80</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6126,7 +6138,7 @@
       <c r="E42" s="6">
         <v>85</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6144,7 +6156,7 @@
       <c r="E43" s="6">
         <v>80</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6162,7 +6174,7 @@
       <c r="E44" s="6">
         <v>80</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6180,7 +6192,7 @@
       <c r="E45" s="6">
         <v>85</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6198,7 +6210,7 @@
       <c r="E46" s="6">
         <v>80</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6216,7 +6228,7 @@
       <c r="E47" s="6">
         <v>75</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6234,7 +6246,7 @@
       <c r="E48" s="6">
         <v>80</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6252,7 +6264,7 @@
       <c r="E49" s="6">
         <v>80</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6270,7 +6282,7 @@
       <c r="E50" s="6">
         <v>80</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6288,7 +6300,7 @@
       <c r="E51" s="6">
         <v>85</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6306,7 +6318,7 @@
       <c r="E52" s="6">
         <v>85</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6324,7 +6336,7 @@
       <c r="E53" s="6">
         <v>105</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -6342,7 +6354,7 @@
       <c r="E54" s="6">
         <v>85</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6360,7 +6372,7 @@
       <c r="E55" s="6">
         <v>80</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6378,7 +6390,7 @@
       <c r="E56" s="6">
         <v>80</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6396,7 +6408,7 @@
       <c r="E57" s="6">
         <v>80</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6414,7 +6426,7 @@
       <c r="E58" s="6">
         <v>200</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -6432,7 +6444,7 @@
       <c r="E59" s="6">
         <v>80</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6450,7 +6462,7 @@
       <c r="E60" s="6">
         <v>80</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6468,7 +6480,7 @@
       <c r="E61" s="6">
         <v>80</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6486,7 +6498,7 @@
       <c r="E62" s="6">
         <v>80</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6504,7 +6516,7 @@
       <c r="E63" s="6">
         <v>85</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6522,7 +6534,7 @@
       <c r="E64" s="6">
         <v>100</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -6540,7 +6552,7 @@
       <c r="E65" s="6">
         <v>75</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6558,7 +6570,7 @@
       <c r="E66" s="6">
         <v>75</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6576,7 +6588,7 @@
       <c r="E67" s="6">
         <v>80</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6594,7 +6606,7 @@
       <c r="E68" s="6">
         <v>85</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6612,7 +6624,7 @@
       <c r="E69" s="6">
         <v>80</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6630,7 +6642,7 @@
       <c r="E70" s="6">
         <v>85</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6648,7 +6660,7 @@
       <c r="E71" s="6">
         <v>80</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6666,7 +6678,7 @@
       <c r="E72" s="6">
         <v>85</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6684,7 +6696,7 @@
       <c r="E73" s="6">
         <v>80</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6702,7 +6714,7 @@
       <c r="E74" s="6">
         <v>80</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6720,7 +6732,7 @@
       <c r="E75" s="6">
         <v>85</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6738,7 +6750,7 @@
       <c r="E76" s="6">
         <v>80</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6756,7 +6768,7 @@
       <c r="E77" s="6">
         <v>85</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6766,6 +6778,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
+      <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
@@ -6781,7 +6794,7 @@
       <c r="E79" s="6">
         <v>85</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6799,7 +6812,7 @@
       <c r="E80" s="6">
         <v>75</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6817,7 +6830,7 @@
       <c r="E81" s="6">
         <v>85</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6835,7 +6848,7 @@
       <c r="E82" s="6">
         <v>100</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -6853,7 +6866,7 @@
       <c r="E83" s="6">
         <v>75</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6873,16 +6886,16 @@
       <c r="E84" s="6">
         <v>75</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="4"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
+      <c r="A85" s="17"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
@@ -10541,6 +10554,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27a4c553-e118-4eca-8f68-9ab2f6bc7790">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="072f65fd-8ac8-4458-b326-98f31ae95622" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056AE81D6219DD048908ADF242EEFC32D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8986bdc60267b136fae45e9c5006776b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="072f65fd-8ac8-4458-b326-98f31ae95622" xmlns:ns3="27a4c553-e118-4eca-8f68-9ab2f6bc7790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3fc11a8a20b827f47d265a4e041875c3" ns2:_="" ns3:_="">
     <xsd:import namespace="072f65fd-8ac8-4458-b326-98f31ae95622"/>
@@ -10775,27 +10808,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2BB9A02-9680-4F30-A06C-9579F93AE1D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27a4c553-e118-4eca-8f68-9ab2f6bc7790"/>
+    <ds:schemaRef ds:uri="072f65fd-8ac8-4458-b326-98f31ae95622"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27a4c553-e118-4eca-8f68-9ab2f6bc7790">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="072f65fd-8ac8-4458-b326-98f31ae95622" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3F43D9-F9A1-4725-A9B7-C5F5F2B8D269}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F96BD55E-408A-4963-8C68-986ACBD01E62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10812,23 +10844,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3F43D9-F9A1-4725-A9B7-C5F5F2B8D269}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2BB9A02-9680-4F30-A06C-9579F93AE1D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27a4c553-e118-4eca-8f68-9ab2f6bc7790"/>
-    <ds:schemaRef ds:uri="072f65fd-8ac8-4458-b326-98f31ae95622"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: total cost not showing on invoice, title of invoice same as filename
</commit_message>
<xml_diff>
--- a/resources/report.xlsx
+++ b/resources/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianguarino/projects/invoice_generator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0EC3DA-2CED-8742-909C-9D39AA2E0896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6723AFAF-67A8-F34C-A2B1-FD3E8E371443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27160" firstSheet="7" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20220" firstSheet="7" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 22" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="191">
   <si>
     <t>UNIT</t>
   </si>
@@ -633,9 +633,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,15 +668,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6137,10 +6146,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6175,6 +6184,7 @@
       <c r="C2">
         <v>1016</v>
       </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2">
         <v>75</v>
       </c>
@@ -6192,6 +6202,7 @@
       <c r="C3">
         <v>1012</v>
       </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2">
         <v>75</v>
       </c>
@@ -6209,6 +6220,7 @@
       <c r="C4">
         <v>1011</v>
       </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2">
         <v>75</v>
       </c>
@@ -6226,6 +6238,7 @@
       <c r="C5">
         <v>1018</v>
       </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2">
         <v>75</v>
       </c>
@@ -6243,6 +6256,7 @@
       <c r="C6">
         <v>986</v>
       </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2">
         <v>75</v>
       </c>
@@ -6260,6 +6274,7 @@
       <c r="C7">
         <v>990</v>
       </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2">
         <v>75</v>
       </c>
@@ -6277,6 +6292,7 @@
       <c r="C8">
         <v>1010</v>
       </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2">
         <v>75</v>
       </c>
@@ -6294,6 +6310,7 @@
       <c r="C9">
         <v>989</v>
       </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2">
         <v>75</v>
       </c>
@@ -6311,6 +6328,7 @@
       <c r="C10">
         <v>1005</v>
       </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2">
         <v>75</v>
       </c>
@@ -6348,6 +6366,7 @@
       <c r="C12">
         <v>1001</v>
       </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2">
         <v>75</v>
       </c>
@@ -6365,6 +6384,7 @@
       <c r="C13">
         <v>996</v>
       </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2">
         <v>75</v>
       </c>
@@ -6382,6 +6402,7 @@
       <c r="C14">
         <v>1017</v>
       </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2">
         <v>75</v>
       </c>
@@ -6399,6 +6420,7 @@
       <c r="C15">
         <v>1004</v>
       </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2">
         <v>75</v>
       </c>
@@ -6419,6 +6441,7 @@
       <c r="D16" s="2">
         <v>100</v>
       </c>
+      <c r="E16" s="2"/>
       <c r="F16" t="s">
         <v>164</v>
       </c>
@@ -6436,6 +6459,7 @@
       <c r="D17" s="2">
         <v>5</v>
       </c>
+      <c r="E17" s="2"/>
       <c r="F17" t="s">
         <v>164</v>
       </c>
@@ -6450,6 +6474,7 @@
       <c r="C18">
         <v>995</v>
       </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2">
         <v>75</v>
       </c>
@@ -6467,6 +6492,7 @@
       <c r="C19">
         <v>985</v>
       </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2">
         <v>75</v>
       </c>
@@ -6484,6 +6510,7 @@
       <c r="C20">
         <v>998</v>
       </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2">
         <v>75</v>
       </c>
@@ -6501,6 +6528,7 @@
       <c r="C21">
         <v>1008</v>
       </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2">
         <v>75</v>
       </c>
@@ -6518,6 +6546,7 @@
       <c r="C22">
         <v>1003</v>
       </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2">
         <v>75</v>
       </c>
@@ -6535,6 +6564,7 @@
       <c r="C23">
         <v>1009</v>
       </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2">
         <v>75</v>
       </c>
@@ -6555,6 +6585,7 @@
       <c r="D24" s="2">
         <v>105</v>
       </c>
+      <c r="E24" s="2"/>
       <c r="F24" t="s">
         <v>164</v>
       </c>
@@ -6589,6 +6620,7 @@
       <c r="C26">
         <v>994</v>
       </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2">
         <v>75</v>
       </c>
@@ -6609,6 +6641,7 @@
       <c r="D27" s="2">
         <v>100</v>
       </c>
+      <c r="E27" s="2"/>
       <c r="F27" t="s">
         <v>164</v>
       </c>
@@ -6626,7 +6659,59 @@
       <c r="D28" s="2">
         <v>100</v>
       </c>
+      <c r="E28" s="2"/>
       <c r="F28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1702</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45554</v>
+      </c>
+      <c r="C29">
+        <v>1020</v>
+      </c>
+      <c r="E29">
+        <v>75</v>
+      </c>
+      <c r="F29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>626</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45555</v>
+      </c>
+      <c r="C30">
+        <v>1041</v>
+      </c>
+      <c r="E30" s="2">
+        <v>75</v>
+      </c>
+      <c r="F30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1927</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45562</v>
+      </c>
+      <c r="C31">
+        <v>1035</v>
+      </c>
+      <c r="D31">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>

<commit_message>
organized functions and paths from index.js to different folders, added main invoice folder generator, fix: date as undefined in the PDF
</commit_message>
<xml_diff>
--- a/resources/report.xlsx
+++ b/resources/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianguarino/projects/invoice_generator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6723AFAF-67A8-F34C-A2B1-FD3E8E371443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F9BAF3-A65C-FB4D-8EAC-11AAF3F0E450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20220" firstSheet="7" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,9 +613,6 @@
     <t>Unit Number</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Invoice Number</t>
   </si>
   <si>
@@ -625,15 +622,19 @@
     <t>Labor Cost</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Invoice Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -674,8 +675,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -6149,26 +6150,33 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>185</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" t="s">
         <v>186</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E1" t="s">
-        <v>189</v>
       </c>
       <c r="F1" t="s">
         <v>190</v>
@@ -6178,14 +6186,13 @@
       <c r="A2">
         <v>222</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>45546</v>
       </c>
       <c r="C2">
         <v>1016</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>75</v>
       </c>
       <c r="F2" t="s">
@@ -6196,14 +6203,13 @@
       <c r="A3">
         <v>328</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>45541</v>
       </c>
       <c r="C3">
         <v>1012</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>75</v>
       </c>
       <c r="F3" t="s">
@@ -6214,14 +6220,13 @@
       <c r="A4">
         <v>502</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>45541</v>
       </c>
       <c r="C4">
         <v>1011</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>75</v>
       </c>
       <c r="F4" t="s">
@@ -6232,14 +6237,13 @@
       <c r="A5">
         <v>605</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>45547</v>
       </c>
       <c r="C5">
         <v>1018</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>75</v>
       </c>
       <c r="F5" t="s">
@@ -6250,14 +6254,13 @@
       <c r="A6">
         <v>626</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>45548</v>
       </c>
       <c r="C6">
         <v>986</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>75</v>
       </c>
       <c r="F6" t="s">
@@ -6268,14 +6271,13 @@
       <c r="A7">
         <v>808</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>45545</v>
       </c>
       <c r="C7">
         <v>990</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>75</v>
       </c>
       <c r="F7" t="s">
@@ -6286,14 +6288,13 @@
       <c r="A8">
         <v>808</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>45541</v>
       </c>
       <c r="C8">
         <v>1010</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>75</v>
       </c>
       <c r="F8" t="s">
@@ -6304,14 +6305,13 @@
       <c r="A9">
         <v>826</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>45545</v>
       </c>
       <c r="C9">
         <v>989</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>75</v>
       </c>
       <c r="F9" t="s">
@@ -6322,14 +6322,13 @@
       <c r="A10">
         <v>827</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>45534</v>
       </c>
       <c r="C10">
         <v>1005</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>75</v>
       </c>
       <c r="F10" t="s">
@@ -6340,16 +6339,16 @@
       <c r="A11">
         <v>928</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>45538</v>
       </c>
       <c r="C11">
         <v>1000</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>150</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>75</v>
       </c>
       <c r="F11" t="s">
@@ -6360,14 +6359,13 @@
       <c r="A12">
         <v>929</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>45538</v>
       </c>
       <c r="C12">
         <v>1001</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>75</v>
       </c>
       <c r="F12" t="s">
@@ -6378,14 +6376,13 @@
       <c r="A13">
         <v>929</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>45538</v>
       </c>
       <c r="C13">
         <v>996</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>75</v>
       </c>
       <c r="F13" t="s">
@@ -6396,14 +6393,13 @@
       <c r="A14">
         <v>1007</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>45547</v>
       </c>
       <c r="C14">
         <v>1017</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>75</v>
       </c>
       <c r="F14" t="s">
@@ -6414,14 +6410,13 @@
       <c r="A15">
         <v>1107</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>45538</v>
       </c>
       <c r="C15">
         <v>1004</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>75</v>
       </c>
       <c r="F15" t="s">
@@ -6432,16 +6427,15 @@
       <c r="A16">
         <v>1123</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>45526</v>
       </c>
       <c r="C16">
         <v>992</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>100</v>
       </c>
-      <c r="E16" s="2"/>
       <c r="F16" t="s">
         <v>164</v>
       </c>
@@ -6450,16 +6444,15 @@
       <c r="A17">
         <v>1126</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>45546</v>
       </c>
       <c r="C17">
         <v>987</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>5</v>
       </c>
-      <c r="E17" s="2"/>
       <c r="F17" t="s">
         <v>164</v>
       </c>
@@ -6468,14 +6461,13 @@
       <c r="A18">
         <v>1321</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>45544</v>
       </c>
       <c r="C18">
         <v>995</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>75</v>
       </c>
       <c r="F18" t="s">
@@ -6486,14 +6478,13 @@
       <c r="A19">
         <v>1329</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>45551</v>
       </c>
       <c r="C19">
         <v>985</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>75</v>
       </c>
       <c r="F19" t="s">
@@ -6504,14 +6495,13 @@
       <c r="A20">
         <v>1402</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>45538</v>
       </c>
       <c r="C20">
         <v>998</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>75</v>
       </c>
       <c r="F20" t="s">
@@ -6522,14 +6512,13 @@
       <c r="A21">
         <v>1526</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>45534</v>
       </c>
       <c r="C21">
         <v>1008</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>75</v>
       </c>
       <c r="F21" t="s">
@@ -6540,14 +6529,13 @@
       <c r="A22">
         <v>1702</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>45538</v>
       </c>
       <c r="C22">
         <v>1003</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>75</v>
       </c>
       <c r="F22" t="s">
@@ -6558,14 +6546,13 @@
       <c r="A23">
         <v>1824</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>45541</v>
       </c>
       <c r="C23">
         <v>1009</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>75</v>
       </c>
       <c r="F23" t="s">
@@ -6576,16 +6563,15 @@
       <c r="A24">
         <v>2005</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>45544</v>
       </c>
       <c r="C24">
         <v>993</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>105</v>
       </c>
-      <c r="E24" s="2"/>
       <c r="F24" t="s">
         <v>164</v>
       </c>
@@ -6594,16 +6580,16 @@
       <c r="A25">
         <v>2201</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>45551</v>
       </c>
       <c r="C25">
         <v>984</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>64</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>75</v>
       </c>
       <c r="F25" t="s">
@@ -6614,14 +6600,13 @@
       <c r="A26">
         <v>2201</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>45544</v>
       </c>
       <c r="C26">
         <v>994</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>75</v>
       </c>
       <c r="F26" t="s">
@@ -6632,16 +6617,15 @@
       <c r="A27">
         <v>2204</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>45534</v>
       </c>
       <c r="C27">
         <v>991</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>100</v>
       </c>
-      <c r="E27" s="2"/>
       <c r="F27" t="s">
         <v>164</v>
       </c>
@@ -6650,16 +6634,15 @@
       <c r="A28">
         <v>2425</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>45553</v>
       </c>
       <c r="C28">
         <v>960</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>100</v>
       </c>
-      <c r="E28" s="2"/>
       <c r="F28" t="s">
         <v>164</v>
       </c>
@@ -6668,13 +6651,13 @@
       <c r="A29">
         <v>1702</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>45554</v>
       </c>
       <c r="C29">
         <v>1020</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>75</v>
       </c>
       <c r="F29" t="s">
@@ -6685,13 +6668,13 @@
       <c r="A30">
         <v>626</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>45555</v>
       </c>
       <c r="C30">
         <v>1041</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>75</v>
       </c>
       <c r="F30" t="s">
@@ -6702,13 +6685,13 @@
       <c r="A31">
         <v>1927</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>45562</v>
       </c>
       <c r="C31">
         <v>1035</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>105</v>
       </c>
       <c r="F31" t="s">
@@ -6718,7 +6701,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 C1:E1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added db functions and cleaned up other .js files
</commit_message>
<xml_diff>
--- a/resources/report.xlsx
+++ b/resources/report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianguarino/projects/invoice_generator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD50AD7E-F127-3144-B46A-CADB804F599C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E14C5E5-999B-8D42-8990-758F16E14A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="3580" windowWidth="34200" windowHeight="22140" firstSheet="5" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20460" firstSheet="7" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 22" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,9 @@
     <sheet name="Sep 24" sheetId="21" r:id="rId21"/>
     <sheet name="Oct 24" sheetId="22" r:id="rId22"/>
     <sheet name="Nov 24" sheetId="23" r:id="rId23"/>
+    <sheet name="Dec 24" sheetId="24" r:id="rId24"/>
+    <sheet name="Jan 25" sheetId="25" r:id="rId25"/>
+    <sheet name="Feb 25" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="241">
   <si>
     <t>UNIT</t>
   </si>
@@ -628,16 +631,199 @@
   </si>
   <si>
     <t>Invoice Type</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Date Sent</t>
+  </si>
+  <si>
+    <t>Payed</t>
+  </si>
+  <si>
+    <t>523F</t>
+  </si>
+  <si>
+    <t>527F</t>
+  </si>
+  <si>
+    <t>528F</t>
+  </si>
+  <si>
+    <t>623F</t>
+  </si>
+  <si>
+    <t>823F</t>
+  </si>
+  <si>
+    <t>928F</t>
+  </si>
+  <si>
+    <t>1121F</t>
+  </si>
+  <si>
+    <t>1123F</t>
+  </si>
+  <si>
+    <t>1227F</t>
+  </si>
+  <si>
+    <t>1323F</t>
+  </si>
+  <si>
+    <t>1328F</t>
+  </si>
+  <si>
+    <t>1629F</t>
+  </si>
+  <si>
+    <t>1726F</t>
+  </si>
+  <si>
+    <t>1822F</t>
+  </si>
+  <si>
+    <t>2025F</t>
+  </si>
+  <si>
+    <t>2028F</t>
+  </si>
+  <si>
+    <t>2127F</t>
+  </si>
+  <si>
+    <t>2226F</t>
+  </si>
+  <si>
+    <t>2227F</t>
+  </si>
+  <si>
+    <t>2322F</t>
+  </si>
+  <si>
+    <t>2427F</t>
+  </si>
+  <si>
+    <t>206F</t>
+  </si>
+  <si>
+    <t>305F</t>
+  </si>
+  <si>
+    <t>321F</t>
+  </si>
+  <si>
+    <t>422F</t>
+  </si>
+  <si>
+    <t>510F</t>
+  </si>
+  <si>
+    <t>514F</t>
+  </si>
+  <si>
+    <t>605F</t>
+  </si>
+  <si>
+    <t>706F</t>
+  </si>
+  <si>
+    <t>808F</t>
+  </si>
+  <si>
+    <t>1107F</t>
+  </si>
+  <si>
+    <t>1124F</t>
+  </si>
+  <si>
+    <t>1209F</t>
+  </si>
+  <si>
+    <t>1304F</t>
+  </si>
+  <si>
+    <t>1406F</t>
+  </si>
+  <si>
+    <t>1501F</t>
+  </si>
+  <si>
+    <t>1601F</t>
+  </si>
+  <si>
+    <t>1605F</t>
+  </si>
+  <si>
+    <t>1606F</t>
+  </si>
+  <si>
+    <t>1609F</t>
+  </si>
+  <si>
+    <t>1706F</t>
+  </si>
+  <si>
+    <t>1801F</t>
+  </si>
+  <si>
+    <t>1808F</t>
+  </si>
+  <si>
+    <t>2102F</t>
+  </si>
+  <si>
+    <t>2103F</t>
+  </si>
+  <si>
+    <t>2202F</t>
+  </si>
+  <si>
+    <t>2208F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,13 +846,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4703,7 +4934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6708,7 +6939,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6975,11 +7208,8 @@
       <c r="D15">
         <v>5</v>
       </c>
-      <c r="E15">
-        <v>75</v>
-      </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -7076,16 +7306,2267 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F20" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F14 A16:F20 A15:D15" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>308</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45615</v>
+      </c>
+      <c r="C2">
+        <v>1093</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>417</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45622</v>
+      </c>
+      <c r="C3">
+        <v>1098</v>
+      </c>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>509</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45608</v>
+      </c>
+      <c r="C4">
+        <v>1090</v>
+      </c>
+      <c r="E4">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>705</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45611</v>
+      </c>
+      <c r="C5">
+        <v>1073</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>809</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45607</v>
+      </c>
+      <c r="C6">
+        <v>1063</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1125</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45616</v>
+      </c>
+      <c r="C7">
+        <v>1095</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1429</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45611</v>
+      </c>
+      <c r="C8">
+        <v>1067</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1527</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45612</v>
+      </c>
+      <c r="C9">
+        <v>1092</v>
+      </c>
+      <c r="E9">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1627</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45596</v>
+      </c>
+      <c r="C10">
+        <v>1060</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1806</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45607</v>
+      </c>
+      <c r="C11">
+        <v>1064</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2102</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45618</v>
+      </c>
+      <c r="C12">
+        <v>1074</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="F12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2121</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45609</v>
+      </c>
+      <c r="C13">
+        <v>1065</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2305</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45596</v>
+      </c>
+      <c r="C14">
+        <v>1087</v>
+      </c>
+      <c r="E14">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:F9 A11:F14 A10:C10 E10:F10" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:I43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>214</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45637</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1104</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>427</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45643</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1108</v>
+      </c>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>523</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45646</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>75</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>527</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45646</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>75</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>528</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45646</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>75</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>623</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45646</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>75</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>627</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45646</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>823</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45645</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>75</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>829</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45645</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>928</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45644</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>75</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1021</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45644</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>75</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1024</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45644</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>75</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1026</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45644</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>75</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1121</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45643</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1123</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45643</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>75</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1123</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45631</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1080</v>
+      </c>
+      <c r="E17">
+        <v>75</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1227</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45643</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>75</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1323</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45642</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>75</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1328</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45642</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>75</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1429</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1082</v>
+      </c>
+      <c r="E21">
+        <v>75</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1521</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45649</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1107</v>
+      </c>
+      <c r="E22">
+        <v>75</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1528</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45639</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>75</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1621</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1081</v>
+      </c>
+      <c r="E24">
+        <v>75</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1624</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45639</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>75</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1629</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45639</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>75</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1629</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45645</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1114</v>
+      </c>
+      <c r="E27">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1702</v>
+      </c>
+      <c r="B28" s="2">
+        <v>45628</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E28">
+        <v>75</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1704</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45628</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1078</v>
+      </c>
+      <c r="E29">
+        <v>75</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1726</v>
+      </c>
+      <c r="B30" s="2">
+        <v>45638</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>75</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1822</v>
+      </c>
+      <c r="B31" s="2">
+        <v>45638</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>75</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1823</v>
+      </c>
+      <c r="B32" s="2">
+        <v>45638</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>75</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="2">
+        <v>45637</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>75</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2028</v>
+      </c>
+      <c r="B34" s="2">
+        <v>45637</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>75</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2126</v>
+      </c>
+      <c r="B35" s="2">
+        <v>45636</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>75</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2127</v>
+      </c>
+      <c r="B36" s="2">
+        <v>45636</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>75</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2226</v>
+      </c>
+      <c r="B37" s="2">
+        <v>45636</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>75</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2227</v>
+      </c>
+      <c r="B38" s="2">
+        <v>45636</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>75</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2321</v>
+      </c>
+      <c r="B39" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>75</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2322</v>
+      </c>
+      <c r="B40" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40">
+        <v>15</v>
+      </c>
+      <c r="E40">
+        <v>75</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2326</v>
+      </c>
+      <c r="B41" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>75</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2421</v>
+      </c>
+      <c r="B42" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>75</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2427</v>
+      </c>
+      <c r="B43" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>75</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:I43" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <dimension ref="A1:I55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>206</v>
+      </c>
+      <c r="B2" s="4">
+        <v>45679</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="3">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>75</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>304</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1144</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>305</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45679</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>75</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>321</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45663</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>75</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>322</v>
+      </c>
+      <c r="B6" s="4">
+        <v>45663</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6">
+        <v>75</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>405</v>
+      </c>
+      <c r="B7" s="4">
+        <v>45679</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6">
+        <v>75</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>407</v>
+      </c>
+      <c r="B8" s="4">
+        <v>45679</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>412</v>
+      </c>
+      <c r="B9" s="4">
+        <v>45679</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>75</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>422</v>
+      </c>
+      <c r="B10" s="4">
+        <v>45663</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="3">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6">
+        <v>75</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>503</v>
+      </c>
+      <c r="B11" s="4">
+        <v>45663</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1120</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="6">
+        <v>75</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>507</v>
+      </c>
+      <c r="B12" s="4">
+        <v>45678</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1127</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+      <c r="E12" s="6">
+        <v>75</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>507</v>
+      </c>
+      <c r="B13" s="4">
+        <v>45681</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1147</v>
+      </c>
+      <c r="D13" s="3">
+        <v>33</v>
+      </c>
+      <c r="E13" s="6">
+        <v>75</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>510</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45674</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="6">
+        <v>75</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>514</v>
+      </c>
+      <c r="B15" s="4">
+        <v>45674</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5</v>
+      </c>
+      <c r="E15" s="6">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>524</v>
+      </c>
+      <c r="B16" s="4">
+        <v>45646</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5</v>
+      </c>
+      <c r="E16" s="6">
+        <v>75</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>604</v>
+      </c>
+      <c r="B17" s="4">
+        <v>45666</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1141</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="6">
+        <v>75</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>605</v>
+      </c>
+      <c r="B18" s="4">
+        <v>45674</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D18" s="3">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6">
+        <v>75</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>703</v>
+      </c>
+      <c r="B19" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6">
+        <v>75</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>706</v>
+      </c>
+      <c r="B20" s="4">
+        <v>45673</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="3">
+        <v>10</v>
+      </c>
+      <c r="E20" s="6">
+        <v>75</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>724</v>
+      </c>
+      <c r="B21" s="4">
+        <v>45679</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1129</v>
+      </c>
+      <c r="D21" s="3">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>808</v>
+      </c>
+      <c r="B22" s="4">
+        <v>45673</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D22" s="3">
+        <v>5</v>
+      </c>
+      <c r="E22" s="6">
+        <v>75</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>1002</v>
+      </c>
+      <c r="B23" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="3">
+        <v>5</v>
+      </c>
+      <c r="E23" s="6">
+        <v>75</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>1006</v>
+      </c>
+      <c r="B24" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="3">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6">
+        <v>75</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>1024</v>
+      </c>
+      <c r="B25" s="4">
+        <v>45652</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1139</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="6">
+        <v>75</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>1107</v>
+      </c>
+      <c r="B26" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="3">
+        <v>5</v>
+      </c>
+      <c r="E26" s="6">
+        <v>75</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>1124</v>
+      </c>
+      <c r="B27" s="4">
+        <v>45643</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5</v>
+      </c>
+      <c r="E27" s="6">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>1129</v>
+      </c>
+      <c r="B28" s="4">
+        <v>45684</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1131</v>
+      </c>
+      <c r="D28" s="3">
+        <v>5</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>1209</v>
+      </c>
+      <c r="B29" s="4">
+        <v>45671</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="3">
+        <v>10</v>
+      </c>
+      <c r="E29" s="6">
+        <v>75</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>1304</v>
+      </c>
+      <c r="B30" s="4">
+        <v>45671</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D30" s="3">
+        <v>5</v>
+      </c>
+      <c r="E30" s="6">
+        <v>75</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>1402</v>
+      </c>
+      <c r="B31" s="4">
+        <v>45671</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="3">
+        <v>5</v>
+      </c>
+      <c r="E31" s="6">
+        <v>75</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>1406</v>
+      </c>
+      <c r="B32" s="4">
+        <v>45671</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D32" s="3">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6">
+        <v>75</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>1501</v>
+      </c>
+      <c r="B33" s="4">
+        <v>45671</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D33" s="3">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6">
+        <v>75</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>1502</v>
+      </c>
+      <c r="B34" s="4">
+        <v>45671</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="3">
+        <v>5</v>
+      </c>
+      <c r="E34" s="6">
+        <v>75</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>1527</v>
+      </c>
+      <c r="B35" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1140</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="6">
+        <v>75</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>1601</v>
+      </c>
+      <c r="B36" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D36" s="3">
+        <v>5</v>
+      </c>
+      <c r="E36" s="6">
+        <v>75</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>1605</v>
+      </c>
+      <c r="B37" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D37" s="3">
+        <v>5</v>
+      </c>
+      <c r="E37" s="6">
+        <v>75</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>1606</v>
+      </c>
+      <c r="B38" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D38" s="3">
+        <v>5</v>
+      </c>
+      <c r="E38" s="6">
+        <v>75</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>1609</v>
+      </c>
+      <c r="B39" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" s="3">
+        <v>5</v>
+      </c>
+      <c r="E39" s="6">
+        <v>75</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>1706</v>
+      </c>
+      <c r="B40" s="4">
+        <v>45672</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5</v>
+      </c>
+      <c r="E40" s="6">
+        <v>75</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>1801</v>
+      </c>
+      <c r="B41" s="4">
+        <v>45666</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D41" s="3">
+        <v>10</v>
+      </c>
+      <c r="E41" s="6">
+        <v>75</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>1808</v>
+      </c>
+      <c r="B42" s="4">
+        <v>45666</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="3">
+        <v>5</v>
+      </c>
+      <c r="E42" s="6">
+        <v>75</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>1902</v>
+      </c>
+      <c r="B43" s="4">
+        <v>45670</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1122</v>
+      </c>
+      <c r="D43" s="3">
+        <v>5</v>
+      </c>
+      <c r="E43" s="6">
+        <v>75</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>2102</v>
+      </c>
+      <c r="B44" s="4">
+        <v>45665</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D44" s="3">
+        <v>5</v>
+      </c>
+      <c r="E44" s="6">
+        <v>75</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>2103</v>
+      </c>
+      <c r="B45" s="4">
+        <v>45665</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D45" s="3">
+        <v>5</v>
+      </c>
+      <c r="E45" s="6">
+        <v>75</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>2104</v>
+      </c>
+      <c r="B46" s="4">
+        <v>45665</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" s="3">
+        <v>5</v>
+      </c>
+      <c r="E46" s="6">
+        <v>75</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>2202</v>
+      </c>
+      <c r="B47" s="4">
+        <v>45665</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="3">
+        <v>10</v>
+      </c>
+      <c r="E47" s="6">
+        <v>75</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>2208</v>
+      </c>
+      <c r="B48" s="4">
+        <v>45665</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D48" s="3">
+        <v>5</v>
+      </c>
+      <c r="E48" s="6">
+        <v>75</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>2225</v>
+      </c>
+      <c r="B49" s="4">
+        <v>45663</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1119</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="6">
+        <v>75</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>2228</v>
+      </c>
+      <c r="B50" s="4">
+        <v>45671</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1143</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="6">
+        <v>75</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>2303</v>
+      </c>
+      <c r="B51" s="4">
+        <v>45664</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="3">
+        <v>5</v>
+      </c>
+      <c r="E51" s="6">
+        <v>75</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>2305</v>
+      </c>
+      <c r="B52" s="4">
+        <v>45664</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="3">
+        <v>5</v>
+      </c>
+      <c r="E52" s="6">
+        <v>75</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>2308</v>
+      </c>
+      <c r="B53" s="4">
+        <v>45664</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53" s="3">
+        <v>5</v>
+      </c>
+      <c r="E53" s="6">
+        <v>75</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>2401</v>
+      </c>
+      <c r="B54" s="4">
+        <v>45664</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D54" s="3">
+        <v>5</v>
+      </c>
+      <c r="E54" s="6">
+        <v>75</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>2406</v>
+      </c>
+      <c r="B55" s="4">
+        <v>45664</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D55" s="3">
+        <v>5</v>
+      </c>
+      <c r="E55" s="6">
+        <v>75</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:I1" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -7107,6 +9588,228 @@
       </c>
       <c r="F1" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>222</v>
+      </c>
+      <c r="B2" s="9">
+        <v>45707</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1157</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13">
+        <v>75</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>304</v>
+      </c>
+      <c r="B3" s="9">
+        <v>45693</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1151</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="14">
+        <v>75</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>312</v>
+      </c>
+      <c r="B4" s="9">
+        <v>45702</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1155</v>
+      </c>
+      <c r="D4" s="15">
+        <v>5</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>522</v>
+      </c>
+      <c r="B5" s="9">
+        <v>45699</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1153</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="14">
+        <v>75</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>527</v>
+      </c>
+      <c r="B6" s="9">
+        <v>45701</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1154</v>
+      </c>
+      <c r="D6" s="17">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17">
+        <v>75</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>626</v>
+      </c>
+      <c r="B7" s="9">
+        <v>45698</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1133</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13">
+        <v>75</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>1107</v>
+      </c>
+      <c r="B8" s="9">
+        <v>45708</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1158</v>
+      </c>
+      <c r="D8" s="15">
+        <v>150</v>
+      </c>
+      <c r="E8" s="13">
+        <v>75</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>1126</v>
+      </c>
+      <c r="B9" s="9">
+        <v>45712</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1160</v>
+      </c>
+      <c r="D9" s="15">
+        <v>100</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>1308</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45712</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1161</v>
+      </c>
+      <c r="D10" s="15">
+        <v>100</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>1401</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45716</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1168</v>
+      </c>
+      <c r="D11" s="15">
+        <v>100</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>1424</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45691</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1135</v>
+      </c>
+      <c r="D12" s="15">
+        <v>70</v>
+      </c>
+      <c r="E12" s="14">
+        <v>75</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>2402</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45714</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1167</v>
+      </c>
+      <c r="D13" s="15">
+        <v>15</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>